<commit_message>
check all, thay đổi ý tưởng csdl, tách modal ra blade riêng để dễ quản lý
</commit_message>
<xml_diff>
--- a/csdl_HaiMocWedding.xlsx
+++ b/csdl_HaiMocWedding.xlsx
@@ -339,7 +339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
   <si>
     <t>Users</t>
   </si>
@@ -486,6 +486,9 @@
   </si>
   <si>
     <t>Roles</t>
+  </si>
+  <si>
+    <t>Services: đổi lại thành id_service, name,bool, icon,mô tả</t>
   </si>
 </sst>
 </file>
@@ -587,9 +590,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -597,6 +597,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -902,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,30 +923,30 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="8" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="H8" s="7" t="s">
+      <c r="E8" s="5"/>
+      <c r="H8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="K8" s="7" t="s">
+      <c r="I8" s="6"/>
+      <c r="K8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="N8" s="7" t="s">
+      <c r="L8" s="6"/>
+      <c r="N8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="7"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
@@ -1086,16 +1089,16 @@
       </c>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="6"/>
+      <c r="L19" s="5"/>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="K20" s="2" t="s">
@@ -1114,22 +1117,22 @@
       </c>
     </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="H29" s="7" t="s">
+      <c r="F29" s="6"/>
+      <c r="H29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="7"/>
-      <c r="K29" s="7" t="s">
+      <c r="I29" s="6"/>
+      <c r="K29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="7"/>
-      <c r="N29" s="5" t="s">
+      <c r="L29" s="6"/>
+      <c r="N29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O29" s="6"/>
+      <c r="O29" s="5"/>
     </row>
     <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
@@ -1244,10 +1247,10 @@
       <c r="F35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="H35" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I35" s="7"/>
+      <c r="I35" s="6"/>
       <c r="K35" s="3" t="s">
         <v>13</v>
       </c>
@@ -1318,6 +1321,9 @@
       </c>
     </row>
     <row r="40" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>49</v>
+      </c>
       <c r="H40" s="1" t="s">
         <v>7</v>
       </c>
@@ -1327,11 +1333,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K19:L19"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D8:E8"/>
@@ -1339,6 +1340,11 @@
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="K29:L29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K19:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CẢI TỔ SERVICE--VẪN CÒN LỖI UPLOAD ICON CHƯA REFRESH
</commit_message>
<xml_diff>
--- a/csdl_HaiMocWedding.xlsx
+++ b/csdl_HaiMocWedding.xlsx
@@ -387,7 +387,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="63">
   <si>
     <t>Users</t>
   </si>
@@ -539,9 +539,6 @@
     <t>Services: đổi lại thành id_service, name, icon</t>
   </si>
   <si>
-    <t>ServicesofPlans</t>
-  </si>
-  <si>
     <t>has_service</t>
   </si>
   <si>
@@ -573,6 +570,12 @@
   </si>
   <si>
     <t>Dịch Vụ này cho những album nào</t>
+  </si>
+  <si>
+    <t>ServicesofAlbums</t>
+  </si>
+  <si>
+    <t>ServicesofPlans(bỏ)</t>
   </si>
 </sst>
 </file>
@@ -697,16 +700,16 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -725,100 +728,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5972175" y="7715250"/>
-          <a:ext cx="704850" cy="561975"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="8362950" y="5495925"/>
-          <a:ext cx="704850" cy="2600325"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
@@ -1029,6 +938,102 @@
         <a:xfrm>
           <a:off x="11610975" y="6753225"/>
           <a:ext cx="85725" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>933451</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>180978</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Elbow Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="2376489" y="5329240"/>
+          <a:ext cx="2724147" cy="1952624"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 93357"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5534025" y="2038350"/>
+          <a:ext cx="590550" cy="2000250"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1346,15 +1351,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -1364,30 +1369,30 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="8" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="H8" s="11" t="s">
+      <c r="E8" s="9"/>
+      <c r="H8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="K8" s="11" t="s">
+      <c r="I8" s="8"/>
+      <c r="K8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="N8" s="11" t="s">
+      <c r="L8" s="8"/>
+      <c r="N8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="11"/>
+      <c r="O8" s="8"/>
     </row>
     <row r="9" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
@@ -1530,20 +1535,20 @@
       </c>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="K19" s="9" t="s">
+      <c r="K19" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="10"/>
+      <c r="L19" s="9"/>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>13</v>
@@ -1554,7 +1559,7 @@
     </row>
     <row r="21" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>34</v>
@@ -1563,23 +1568,61 @@
         <v>8</v>
       </c>
     </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F22" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="E29" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="11"/>
-      <c r="H29" s="11" t="s">
+      <c r="E29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="H29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="11"/>
-      <c r="K29" s="11" t="s">
+      <c r="I29" s="8"/>
+      <c r="K29" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="11"/>
-      <c r="N29" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="O29" s="10"/>
+      <c r="L29" s="8"/>
+      <c r="N29" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="O29" s="9"/>
     </row>
     <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
@@ -1694,10 +1737,10 @@
       <c r="F35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H35" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I35" s="11"/>
+      <c r="I35" s="8"/>
       <c r="K35" s="3" t="s">
         <v>13</v>
       </c>
@@ -1725,12 +1768,12 @@
         <v>8</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N36" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N36" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O36" s="10"/>
+      <c r="O36" s="9"/>
     </row>
     <row r="37" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E37" s="1" t="s">
@@ -1752,7 +1795,7 @@
         <v>8</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>39</v>
@@ -1801,10 +1844,10 @@
       </c>
     </row>
     <row r="41" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F41" s="10"/>
+      <c r="F41" s="9"/>
     </row>
     <row r="42" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E42" s="2" t="s">
@@ -1813,14 +1856,14 @@
       <c r="F42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H42" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I42" s="11"/>
-      <c r="N42" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="O42" s="11"/>
+      <c r="H42" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I42" s="8"/>
+      <c r="N42" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O42" s="8"/>
     </row>
     <row r="43" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E43" s="1" t="s">
@@ -1844,7 +1887,7 @@
     </row>
     <row r="44" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E44" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>10</v>
@@ -1864,16 +1907,16 @@
     </row>
     <row r="45" spans="5:15" x14ac:dyDescent="0.25">
       <c r="H45" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O45" s="1" t="s">
         <v>27</v>
@@ -1887,18 +1930,11 @@
         <v>9</v>
       </c>
       <c r="J46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N36:O36"/>
+  <mergeCells count="17">
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="H35:I35"/>
@@ -1908,6 +1944,14 @@
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="K29:L29"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="N36:O36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>